<commit_message>
Day 1 Questions completed
</commit_message>
<xml_diff>
--- a/Striver SDE.xlsx
+++ b/Striver SDE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding - Striver DSA CP &amp; Love Babbar DSA\Striver SDE Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0AC4D-CE82-4E92-8A00-C59DFD1F1BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB81C94-2643-4208-9F4F-7FDD1AE4D720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">All the Questions and Solutions are of SDE Sheer of striver_79 (take U forward) (striver_79) </t>
   </si>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/sort-colors/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-a-repeating-and-a-missing-number/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat and Missing Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge two sorted Arrays without extra space </t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/efficiently-merging-two-sorted-arrays-with-o1-extra-space/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/largest-sum-contiguous-subarray/</t>
+  </si>
+  <si>
+    <t>Kadane's algorithm</t>
+  </si>
+  <si>
+    <t>Merge Overlapping Subintervals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/</t>
   </si>
 </sst>
 </file>
@@ -71,12 +95,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,16 +121,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,47 +412,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -435,14 +466,52 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Done with Day 10
</commit_message>
<xml_diff>
--- a/Striver SDE.xlsx
+++ b/Striver SDE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding - Striver DSA CP &amp; Love Babbar DSA\Striver SDE Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219928F5-5BB1-43AC-AC15-B899F26F86CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E777D2-F3B9-4751-838E-42E22FBC8C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t xml:space="preserve">All the Questions and Solutions are of SDE Sheer of striver_79 (take U forward) (striver_79) </t>
   </si>
@@ -395,6 +395,33 @@
   </si>
   <si>
     <t>Word Break</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/combination-sum-1587115620/1</t>
+  </si>
+  <si>
+    <t>Day 10</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-ii/</t>
+  </si>
+  <si>
+    <t>Combination Sum 2</t>
+  </si>
+  <si>
+    <t>Combination Sum 1</t>
+  </si>
+  <si>
+    <t>K-th Permutation Sequence</t>
+  </si>
+  <si>
+    <t>Subset Sum 1</t>
+  </si>
+  <si>
+    <t>Subset Sum 2</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning</t>
   </si>
 </sst>
 </file>
@@ -460,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +518,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -505,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -523,11 +556,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -809,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z73"/>
+  <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,34 +858,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1336,7 +1371,7 @@
       <c r="A69" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C69" s="3"/>
@@ -1354,7 +1389,7 @@
       <c r="A71" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C71" s="3"/>
@@ -1375,7 +1410,58 @@
       <c r="B73" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C73" s="15"/>
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="15"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="15"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="14"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Done with Day 11
</commit_message>
<xml_diff>
--- a/Striver SDE.xlsx
+++ b/Striver SDE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding - Striver DSA CP &amp; Love Babbar DSA\Striver SDE Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E777D2-F3B9-4751-838E-42E22FBC8C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87C8BF-FFC9-4BEE-A8B9-172EEE429ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t xml:space="preserve">All the Questions and Solutions are of SDE Sheer of striver_79 (take U forward) (striver_79) </t>
   </si>
@@ -422,6 +422,30 @@
   </si>
   <si>
     <t>Palindrome Partitioning</t>
+  </si>
+  <si>
+    <t>Day 11</t>
+  </si>
+  <si>
+    <t>N-th root of a number</t>
+  </si>
+  <si>
+    <t>Matrix Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the element that appears once in sorted array, and rest element appears twice (Binary search) </t>
+  </si>
+  <si>
+    <t>Search element in a sorted and rotated array</t>
+  </si>
+  <si>
+    <t>Median of 2 sorted arrays</t>
+  </si>
+  <si>
+    <t>K-th element of 2 sorted arrays</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/find-the-element-that-appears-once-in-sorted-array0624/1</t>
   </si>
 </sst>
 </file>
@@ -559,10 +583,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,48 +868,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z81"/>
+  <dimension ref="A1:Z89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="86.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="95.7109375" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1457,11 +1481,56 @@
       </c>
       <c r="C80" s="8"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C81" s="17"/>
+      <c r="C81" s="16"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" s="8"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Done with Day 12
</commit_message>
<xml_diff>
--- a/Striver SDE.xlsx
+++ b/Striver SDE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding - Striver DSA CP &amp; Love Babbar DSA\Striver SDE Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87C8BF-FFC9-4BEE-A8B9-172EEE429ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6706A5-D29C-4C9E-81CC-57BCA84C78BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t xml:space="preserve">All the Questions and Solutions are of SDE Sheer of striver_79 (take U forward) (striver_79) </t>
   </si>
@@ -446,6 +446,30 @@
   </si>
   <si>
     <t>https://practice.geeksforgeeks.org/problems/find-the-element-that-appears-once-in-sorted-array0624/1</t>
+  </si>
+  <si>
+    <t>Day 12</t>
+  </si>
+  <si>
+    <t>Divide two integers without using multiplication, division, and mod operator.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/divide-two-integers/</t>
+  </si>
+  <si>
+    <t>Check Power of 2</t>
+  </si>
+  <si>
+    <t>Count set bits</t>
+  </si>
+  <si>
+    <t>Power set</t>
+  </si>
+  <si>
+    <t>MSB in O(1)</t>
+  </si>
+  <si>
+    <t>Square a number without multiplication or division operators</t>
   </si>
 </sst>
 </file>
@@ -868,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z89"/>
+  <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,6 +1556,50 @@
       </c>
       <c r="C89" s="16"/>
     </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C92" s="8"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94" s="8"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" s="8"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96" s="8"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:Z1"/>

</xml_diff>